<commit_message>
update limit hutang d dalam SO
</commit_message>
<xml_diff>
--- a/storage/exports/so-form-format.xlsx
+++ b/storage/exports/so-form-format.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">SO Code</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">TOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limit</t>
   </si>
   <si>
     <t xml:space="preserve">DateRegister</t>
@@ -304,29 +307,27 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1:N2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="1.94387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="1.88775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,10 +374,12 @@
       <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AMB1" s="0"/>
+      <c r="S1" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="AMC1" s="0"/>
       <c r="AMD1" s="0"/>
       <c r="AME1" s="0"/>
@@ -391,13 +394,13 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
@@ -410,8 +413,8 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="2"/>
-      <c r="AMB2" s="0"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="2"/>
       <c r="AMC2" s="0"/>
       <c r="AMD2" s="0"/>
       <c r="AME2" s="0"/>
@@ -422,7 +425,7 @@
       <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -437,6 +440,7 @@
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update SO and export
</commit_message>
<xml_diff>
--- a/storage/exports/so-form-format.xlsx
+++ b/storage/exports/so-form-format.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">SO Code</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">FinalTotal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Label</t>
   </si>
   <si>
     <t xml:space="preserve">Packing Kayu</t>
@@ -311,29 +314,28 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.91836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="1.75510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="1.62244897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="13" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,10 +388,12 @@
       <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AMD1" s="0"/>
+      <c r="U1" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -403,13 +407,13 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
@@ -423,8 +427,8 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="2"/>
-      <c r="AMD2" s="0"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="2"/>
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
       <c r="AMG2" s="0"/>
@@ -433,7 +437,7 @@
       <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -450,6 +454,7 @@
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>